<commit_message>
update resampling based simulation, automate model running process
</commit_message>
<xml_diff>
--- a/simulate_data/resampling/summary of results.xlsx
+++ b/simulate_data/resampling/summary of results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>catch assumption</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Small amount of noise, 1 stn per strat provides sufficient data for estimating conversion except for large lengths</t>
   </si>
   <si>
-    <t>mu_flatness</t>
-  </si>
-  <si>
     <t>#Senario</t>
   </si>
   <si>
@@ -137,7 +134,43 @@
     <t>ln(p/1-p)=-0.5+0.04*len</t>
   </si>
   <si>
-    <t>ln(p/1-p)=-0.5+0.04*len+error(stn,len)</t>
+    <t>pois(lognormal(dbeta(len,0.5,0.5)))</t>
+  </si>
+  <si>
+    <t>True conversion simple and smooth. More noisy observations than #2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A bit more noise than #1 and heteroskedastic (phi bowl-shaped).  </t>
+  </si>
+  <si>
+    <t>len_sd</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>True conversion dipersed over stations (but still smooth).</t>
+  </si>
+  <si>
+    <t>mu_lin</t>
+  </si>
+  <si>
+    <t>ln(p/1-p)=-0.5*LN(0.3)+0.04*LN(0.3)*len</t>
+  </si>
+  <si>
+    <t>pois(lognormal(dbeta(len,0.8,0.8)))</t>
+  </si>
+  <si>
+    <t>pois(lognormal(0.4))</t>
+  </si>
+  <si>
+    <t>ln(p/1-p)=2*LN(0.3)+0.03*LN(0.3)*len</t>
+  </si>
+  <si>
+    <t>Targeted tows in a list of abundant strata.</t>
+  </si>
+  <si>
+    <t>Biomass Loss (Med)</t>
   </si>
 </sst>
 </file>
@@ -249,43 +282,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X20"/>
+  <dimension ref="A1:Z20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="Y3" sqref="Y3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,120 +625,129 @@
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
     <col min="4" max="4" width="42.140625" customWidth="1"/>
     <col min="5" max="5" width="38.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="24" max="24" width="76.140625" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="25" max="25" width="25.140625" customWidth="1"/>
+    <col min="26" max="26" width="76.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="3" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="9" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="1:26" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="T2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="U2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="V2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="X2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="Y2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -704,12 +758,12 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="10">
         <v>1</v>
       </c>
       <c r="G3">
@@ -718,170 +772,432 @@
       <c r="H3">
         <v>0.30410600998342102</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>0.134458913239795</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>2.9202568417223899E-2</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>2.9203882610312398E-2</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>6.65525733264346E-3</v>
       </c>
-      <c r="M3">
+      <c r="N3">
         <v>6.5862279133404502E-3</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>6.6847427113480096E-3</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>6.5449802768058202E-3</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>6.8631918925241E-3</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>6.96239294227728E-3</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>2.9207369749593801E-2</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>2.92005380459886E-2</v>
       </c>
-      <c r="T3">
+      <c r="U3">
         <v>6.53914862619234E-3</v>
       </c>
-      <c r="U3">
+      <c r="V3">
         <v>6.5542750889134799E-3</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>6.6129652527130902E-3</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>6.8264804076476797E-3</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="Z3" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="10">
         <v>1</v>
       </c>
-      <c r="X4" s="11"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0.50902905982905999</v>
+      </c>
+      <c r="H4">
+        <v>0.32092206699394998</v>
+      </c>
+      <c r="J4">
+        <v>0.134458913239795</v>
+      </c>
+      <c r="K4">
+        <v>2.7996406562268199E-2</v>
+      </c>
+      <c r="L4">
+        <v>2.7998143676523101E-2</v>
+      </c>
+      <c r="M4">
+        <v>1.19778899240266E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.3866143857850901E-2</v>
+      </c>
+      <c r="O4">
+        <v>1.2156520419651E-2</v>
+      </c>
+      <c r="P4">
+        <v>1.4167765352556899E-2</v>
+      </c>
+      <c r="Q4">
+        <v>1.39886665316884E-2</v>
+      </c>
+      <c r="R4">
+        <v>1.6285874909111299E-2</v>
+      </c>
+      <c r="S4">
+        <v>2.8161648084643401E-2</v>
+      </c>
+      <c r="T4">
+        <v>2.8053513501324699E-2</v>
+      </c>
+      <c r="U4">
+        <v>1.0446982389537901E-2</v>
+      </c>
+      <c r="V4">
+        <v>1.03586563163383E-2</v>
+      </c>
+      <c r="W4">
+        <v>1.0097394560295601E-2</v>
+      </c>
+      <c r="X4">
+        <v>1.2982041351130199E-2</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="10">
         <v>2</v>
       </c>
-      <c r="X5" s="11"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F6" s="1">
+      <c r="G5">
+        <v>0.48112991452991499</v>
+      </c>
+      <c r="H5">
+        <v>0.339549231247465</v>
+      </c>
+      <c r="J5">
+        <v>0.21823523416845</v>
+      </c>
+      <c r="K5">
+        <v>5.0402493904260298E-2</v>
+      </c>
+      <c r="L5">
+        <v>5.0109576082388897E-2</v>
+      </c>
+      <c r="M5">
+        <v>9.7073494562231605E-3</v>
+      </c>
+      <c r="N5">
+        <v>7.1414648932942304E-3</v>
+      </c>
+      <c r="O5">
+        <v>9.7832957947100001E-3</v>
+      </c>
+      <c r="P5">
+        <v>6.8384237293069201E-3</v>
+      </c>
+      <c r="Q5">
+        <v>1.02442259998751E-2</v>
+      </c>
+      <c r="R5">
+        <v>7.4342390769153504E-3</v>
+      </c>
+      <c r="S5">
+        <v>5.2056229231414203E-2</v>
+      </c>
+      <c r="T5">
+        <v>4.9392602266086702E-2</v>
+      </c>
+      <c r="U5">
+        <v>1.02833457182143E-2</v>
+      </c>
+      <c r="V5">
+        <v>9.4221795794096307E-3</v>
+      </c>
+      <c r="W5">
+        <v>6.7486400491643204E-3</v>
+      </c>
+      <c r="X5">
+        <v>8.0977944589169706E-3</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="X6" s="11"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="X7" s="11"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X8" s="11"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X9" s="11"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0.47479145299145298</v>
+      </c>
+      <c r="H6">
+        <v>0.34574652359834201</v>
+      </c>
+      <c r="I6">
+        <v>0.35211587744466999</v>
+      </c>
+      <c r="J6">
+        <v>3.5775872510497297E-2</v>
+      </c>
+      <c r="K6">
+        <v>9.5537834402893304E-2</v>
+      </c>
+      <c r="L6">
+        <v>9.4460380558863993E-2</v>
+      </c>
+      <c r="M6">
+        <v>1.5884899178882899E-2</v>
+      </c>
+      <c r="N6">
+        <v>1.2979383887445999E-2</v>
+      </c>
+      <c r="O6">
+        <v>1.3912996329311001E-2</v>
+      </c>
+      <c r="P6">
+        <v>1.17600897931576E-2</v>
+      </c>
+      <c r="Q6">
+        <v>1.3140476418458899E-2</v>
+      </c>
+      <c r="R6">
+        <v>1.0626151141927999E-2</v>
+      </c>
+      <c r="S6">
+        <v>9.8091549333579595E-2</v>
+      </c>
+      <c r="T6">
+        <v>9.2802822862953896E-2</v>
+      </c>
+      <c r="U6">
+        <v>2.7642890690945901E-2</v>
+      </c>
+      <c r="V6">
+        <v>2.3099366987225398E-2</v>
+      </c>
+      <c r="W6">
+        <v>1.6856160226486599E-2</v>
+      </c>
+      <c r="X6">
+        <v>1.25503187489494E-2</v>
+      </c>
+      <c r="Z6" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z7" s="8"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z8" s="8"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z9" s="8"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
       <c r="B10" s="1">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0.140766414141414</v>
+      </c>
+      <c r="H10">
+        <v>0.28928374867360901</v>
+      </c>
+      <c r="I10">
+        <v>0.26367166707424</v>
+      </c>
+      <c r="J10">
+        <v>2.56602410505525E-2</v>
+      </c>
+      <c r="K10">
+        <v>5.25381619029704E-2</v>
+      </c>
+      <c r="L10">
+        <v>5.1912209659132798E-2</v>
+      </c>
+      <c r="M10">
+        <v>1.6491421701801699E-2</v>
+      </c>
+      <c r="N10">
+        <v>1.62421544322339E-2</v>
+      </c>
+      <c r="O10">
+        <v>1.6223105743925399E-2</v>
+      </c>
+      <c r="P10">
+        <v>1.5851936602871299E-2</v>
+      </c>
+      <c r="Q10">
+        <v>1.5751223072541499E-2</v>
+      </c>
+      <c r="R10">
+        <v>1.3954135638087201E-2</v>
+      </c>
+      <c r="S10">
+        <v>5.0352208601420902E-2</v>
+      </c>
+      <c r="T10">
+        <v>5.0373081952816999E-2</v>
+      </c>
+      <c r="U10">
+        <v>1.43688559948304E-2</v>
+      </c>
+      <c r="V10">
+        <v>1.4297159046952701E-2</v>
+      </c>
+      <c r="W10">
+        <v>1.20374761252774E-2</v>
+      </c>
+      <c r="X10">
+        <v>1.7478637064442099E-2</v>
+      </c>
+      <c r="Z10" s="8"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F11" s="10">
         <v>2</v>
       </c>
-      <c r="X10" s="11"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F11" s="1">
+      <c r="Z11" s="8"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="16">
         <v>2</v>
       </c>
-      <c r="X11" s="11"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F12" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="X12" s="11"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F13" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="X13" s="11"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F14" s="1">
-        <v>3</v>
-      </c>
-      <c r="X14" s="11"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X15" s="11"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="X16" s="11"/>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B17" s="1">
+      <c r="Z12" s="8"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="F13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z13" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z14" s="8"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1">
         <v>23</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
+      <c r="C16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="8"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>12</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="X17" s="11"/>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="X18" s="11"/>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="X19" s="11"/>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="X20" s="11"/>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z18" s="8"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z19" s="8"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="Z20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="J1:W1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:X1"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>

</xml_diff>